<commit_message>
add in new lookups and make work
</commit_message>
<xml_diff>
--- a/Data/1-2_LEPmissing/missing_leps.xlsx
+++ b/Data/1-2_LEPmissing/missing_leps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/2_LEPmissing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/1-2_LEPmissing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{FFE31EE7-898F-4126-9D75-02FABA5FEDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E64F47E3-6B29-4117-AB13-8086E583E699}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{FFE31EE7-898F-4126-9D75-02FABA5FEDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54B1BC4F-2070-41B5-BFAB-C5883C1EE999}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="2" xr2:uid="{1E32C2D0-1FE1-4979-B264-7DA23B5223C8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{1E32C2D0-1FE1-4979-B264-7DA23B5223C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sources" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">LADs!$A$1:$D$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">LADs!$A$1:$D$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="109">
   <si>
     <t>time_period</t>
   </si>
@@ -328,13 +328,52 @@
   </si>
   <si>
     <t>UTLA21 map</t>
+  </si>
+  <si>
+    <t>E07000027</t>
+  </si>
+  <si>
+    <t>Barrow-in-Furness</t>
+  </si>
+  <si>
+    <t>E07000030</t>
+  </si>
+  <si>
+    <t>Eden</t>
+  </si>
+  <si>
+    <t>E07000031</t>
+  </si>
+  <si>
+    <t>South Lakeland</t>
+  </si>
+  <si>
+    <t>E07000026</t>
+  </si>
+  <si>
+    <t>Allerdale</t>
+  </si>
+  <si>
+    <t>E07000028</t>
+  </si>
+  <si>
+    <t>Carlisle</t>
+  </si>
+  <si>
+    <t>E07000029</t>
+  </si>
+  <si>
+    <t>Copeland</t>
+  </si>
+  <si>
+    <t>Cumbria</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,6 +399,19 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF323132"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF323132"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -400,13 +452,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -8469,10 +8523,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63CCF82A-C657-4D4C-8BFB-87C91102109C}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27:F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9029,87 +9083,189 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>65</v>
+      <c r="A27" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="B27">
-        <v>201718</v>
-      </c>
-      <c r="C27">
-        <f>SUMIFS(Data!H:H,Data!A:A,LADs!B27,Data!B:B,LADs!A27)</f>
-        <v>39600</v>
-      </c>
-      <c r="E27" t="str">
-        <f>INDEX(Data!C:C,MATCH(LADs!A27,Data!B:B,0))</f>
-        <v>z</v>
+        <v>202122</v>
+      </c>
+      <c r="C27" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="B28">
-        <v>201819</v>
-      </c>
-      <c r="C28">
-        <f>SUMIFS(Data!H:H,Data!A:A,LADs!B28,Data!B:B,LADs!A28)</f>
-        <v>32930</v>
-      </c>
-      <c r="E28" t="str">
-        <f>INDEX(Data!C:C,MATCH(LADs!A28,Data!B:B,0))</f>
-        <v>z</v>
+        <v>202122</v>
+      </c>
+      <c r="C28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>65</v>
+      <c r="A29" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="B29">
-        <v>201920</v>
-      </c>
-      <c r="C29">
-        <f>SUMIFS(Data!H:H,Data!A:A,LADs!B29,Data!B:B,LADs!A29)</f>
-        <v>7230</v>
-      </c>
-      <c r="E29" t="str">
-        <f>INDEX(Data!C:C,MATCH(LADs!A29,Data!B:B,0))</f>
-        <v>z</v>
+        <v>202122</v>
+      </c>
+      <c r="C29" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>65</v>
+      <c r="A30" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="B30">
-        <v>202021</v>
-      </c>
-      <c r="C30">
-        <f>SUMIFS(Data!H:H,Data!A:A,LADs!B30,Data!B:B,LADs!A30)</f>
-        <v>7200</v>
-      </c>
-      <c r="E30" t="str">
-        <f>INDEX(Data!C:C,MATCH(LADs!A30,Data!B:B,0))</f>
-        <v>z</v>
+        <v>202122</v>
+      </c>
+      <c r="C30" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>65</v>
+      <c r="A31" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="B31">
         <v>202122</v>
       </c>
-      <c r="C31">
-        <f>SUMIFS(Data!H:H,Data!A:A,LADs!B31,Data!B:B,LADs!A31)</f>
+      <c r="C31" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32">
+        <v>202122</v>
+      </c>
+      <c r="C32" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33">
+        <v>201718</v>
+      </c>
+      <c r="C33">
+        <f>SUMIFS(Data!H:H,Data!A:A,LADs!B33,Data!B:B,LADs!A33)</f>
+        <v>39600</v>
+      </c>
+      <c r="E33" t="str">
+        <f>INDEX(Data!C:C,MATCH(LADs!A33,Data!B:B,0))</f>
+        <v>z</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34">
+        <v>201819</v>
+      </c>
+      <c r="C34">
+        <f>SUMIFS(Data!H:H,Data!A:A,LADs!B34,Data!B:B,LADs!A34)</f>
+        <v>32930</v>
+      </c>
+      <c r="E34" t="str">
+        <f>INDEX(Data!C:C,MATCH(LADs!A34,Data!B:B,0))</f>
+        <v>z</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35">
+        <v>201920</v>
+      </c>
+      <c r="C35">
+        <f>SUMIFS(Data!H:H,Data!A:A,LADs!B35,Data!B:B,LADs!A35)</f>
+        <v>7230</v>
+      </c>
+      <c r="E35" t="str">
+        <f>INDEX(Data!C:C,MATCH(LADs!A35,Data!B:B,0))</f>
+        <v>z</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36">
+        <v>202021</v>
+      </c>
+      <c r="C36">
+        <f>SUMIFS(Data!H:H,Data!A:A,LADs!B36,Data!B:B,LADs!A36)</f>
+        <v>7200</v>
+      </c>
+      <c r="E36" t="str">
+        <f>INDEX(Data!C:C,MATCH(LADs!A36,Data!B:B,0))</f>
+        <v>z</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37">
+        <v>202122</v>
+      </c>
+      <c r="C37">
+        <f>SUMIFS(Data!H:H,Data!A:A,LADs!B37,Data!B:B,LADs!A37)</f>
         <v>2460</v>
       </c>
-      <c r="E31" t="str">
-        <f>INDEX(Data!C:C,MATCH(LADs!A31,Data!B:B,0))</f>
+      <c r="E37" t="str">
+        <f>INDEX(Data!C:C,MATCH(LADs!A37,Data!B:B,0))</f>
         <v>z</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D27" xr:uid="{63CCF82A-C657-4D4C-8BFB-87C91102109C}"/>
+  <autoFilter ref="A1:D33" xr:uid="{63CCF82A-C657-4D4C-8BFB-87C91102109C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -9119,7 +9275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD77C0D9-0462-4E4B-AB1C-15D5B966B872}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updtae all the maps
</commit_message>
<xml_diff>
--- a/Data/1-2_LEPmissing/missing_leps.xlsx
+++ b/Data/1-2_LEPmissing/missing_leps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/1-2_LEPmissing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{FFE31EE7-898F-4126-9D75-02FABA5FEDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54B1BC4F-2070-41B5-BFAB-C5883C1EE999}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{FFE31EE7-898F-4126-9D75-02FABA5FEDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9ED972DF-E4B2-45E8-88A1-A2D756D8276C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{1E32C2D0-1FE1-4979-B264-7DA23B5223C8}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sources" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">LADs!$A$1:$D$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1">LADs!$A$1:$E$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="118">
   <si>
     <t>time_period</t>
   </si>
@@ -258,9 +258,6 @@
     <t>Local Authority Districts, Counties and Unitary Authorities (December 2017) Map in United Kingdom | Open Geography Portal (statistics.gov.uk)</t>
   </si>
   <si>
-    <t>LEP21 (manually mapped)</t>
-  </si>
-  <si>
     <t>suffolk (east of cambridge)</t>
   </si>
   <si>
@@ -309,12 +306,6 @@
     <t>around northampton</t>
   </si>
   <si>
-    <t xml:space="preserve">LAD21CD </t>
-  </si>
-  <si>
-    <t>LSIP21 (manually mapped)</t>
-  </si>
-  <si>
     <t>Norfolk and Suffolk (Greater Anglia)</t>
   </si>
   <si>
@@ -367,13 +358,49 @@
   </si>
   <si>
     <t>Cumbria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LADCD </t>
+  </si>
+  <si>
+    <t>Cumberland</t>
+  </si>
+  <si>
+    <t>E06000063</t>
+  </si>
+  <si>
+    <t>Westmorland and Furness</t>
+  </si>
+  <si>
+    <t>E06000064</t>
+  </si>
+  <si>
+    <t>LAD23NM</t>
+  </si>
+  <si>
+    <t>LADNM</t>
+  </si>
+  <si>
+    <t>LAD23CD</t>
+  </si>
+  <si>
+    <t>LSIP</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Manual</t>
+  </si>
+  <si>
+    <t>Lookup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,6 +442,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF323132"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -452,7 +485,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -461,6 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -8523,749 +8557,867 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63CCF82A-C657-4D4C-8BFB-87C91102109C}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27:F32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27:I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32.26953125" customWidth="1"/>
-    <col min="3" max="3" width="36.1796875" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.1796875" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
-      <c r="B2">
-        <v>201718</v>
-      </c>
-      <c r="C2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" t="str">
+      <c r="B2" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A2,Data!B:B,0))</f>
         <v>E07000201</v>
       </c>
+      <c r="C2">
+        <v>201718</v>
+      </c>
+      <c r="D2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" t="s">
+        <v>73</v>
+      </c>
       <c r="F2" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+      <c r="I2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>31</v>
       </c>
-      <c r="B3">
-        <v>201718</v>
-      </c>
-      <c r="C3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" t="str">
+      <c r="B3" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A3,Data!B:B,0))</f>
         <v>E07000204</v>
       </c>
+      <c r="C3">
+        <v>201718</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s">
+        <v>73</v>
+      </c>
       <c r="F3" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+      <c r="I3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>33</v>
       </c>
-      <c r="B4">
-        <v>201718</v>
-      </c>
-      <c r="C4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" t="str">
+      <c r="B4" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A4,Data!B:B,0))</f>
         <v>E07000205</v>
       </c>
+      <c r="C4">
+        <v>201718</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s">
+        <v>73</v>
+      </c>
       <c r="F4" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+      <c r="I4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>35</v>
       </c>
-      <c r="B5">
-        <v>201718</v>
-      </c>
-      <c r="C5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" t="str">
+      <c r="B5" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A5,Data!B:B,0))</f>
         <v>E07000206</v>
       </c>
+      <c r="C5">
+        <v>201718</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" t="s">
+        <v>73</v>
+      </c>
       <c r="F5" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+      <c r="I5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>45</v>
       </c>
-      <c r="B6">
-        <v>201718</v>
-      </c>
-      <c r="C6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" t="str">
+      <c r="B6" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A6,Data!B:B,0))</f>
         <v>E06000028</v>
       </c>
+      <c r="C6">
+        <v>201718</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" t="s">
+        <v>74</v>
+      </c>
       <c r="F6" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="I6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>47</v>
       </c>
-      <c r="B7">
-        <v>201718</v>
-      </c>
-      <c r="C7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" t="str">
+      <c r="B7" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A7,Data!B:B,0))</f>
         <v>E07000048</v>
       </c>
+      <c r="C7">
+        <v>201718</v>
+      </c>
+      <c r="D7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" t="s">
+        <v>74</v>
+      </c>
       <c r="F7" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="I7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>49</v>
       </c>
-      <c r="B8">
-        <v>201718</v>
-      </c>
-      <c r="C8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" t="str">
+      <c r="B8" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A8,Data!B:B,0))</f>
         <v>E07000049</v>
       </c>
+      <c r="C8">
+        <v>201718</v>
+      </c>
+      <c r="D8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" t="s">
+        <v>74</v>
+      </c>
       <c r="F8" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="I8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>51</v>
       </c>
-      <c r="B9">
-        <v>201718</v>
-      </c>
-      <c r="C9" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" t="str">
+      <c r="B9" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A9,Data!B:B,0))</f>
         <v>E07000050</v>
       </c>
+      <c r="C9">
+        <v>201718</v>
+      </c>
+      <c r="D9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" t="s">
+        <v>74</v>
+      </c>
       <c r="F9" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="I9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>53</v>
       </c>
-      <c r="B10">
-        <v>201718</v>
-      </c>
-      <c r="C10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" t="str">
+      <c r="B10" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A10,Data!B:B,0))</f>
         <v>E06000029</v>
       </c>
+      <c r="C10">
+        <v>201718</v>
+      </c>
+      <c r="D10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" t="s">
+        <v>74</v>
+      </c>
       <c r="F10" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="I10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>55</v>
       </c>
-      <c r="B11">
-        <v>201718</v>
-      </c>
-      <c r="C11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" t="str">
+      <c r="B11" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A11,Data!B:B,0))</f>
         <v>E07000051</v>
       </c>
+      <c r="C11">
+        <v>201718</v>
+      </c>
+      <c r="D11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" t="s">
+        <v>74</v>
+      </c>
       <c r="F11" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="I11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>57</v>
       </c>
-      <c r="B12">
-        <v>201718</v>
-      </c>
-      <c r="C12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" t="str">
+      <c r="B12" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A12,Data!B:B,0))</f>
         <v>E07000190</v>
       </c>
+      <c r="C12">
+        <v>201718</v>
+      </c>
+      <c r="D12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" t="s">
+        <v>75</v>
+      </c>
       <c r="F12" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+      <c r="I12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>59</v>
       </c>
-      <c r="B13">
-        <v>201718</v>
-      </c>
-      <c r="C13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" t="str">
+      <c r="B13" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A13,Data!B:B,0))</f>
         <v>E07000052</v>
       </c>
+      <c r="C13">
+        <v>201718</v>
+      </c>
+      <c r="D13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" t="s">
+        <v>74</v>
+      </c>
       <c r="F13" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="I13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>61</v>
       </c>
-      <c r="B14">
-        <v>201718</v>
-      </c>
-      <c r="C14" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" t="str">
+      <c r="B14" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A14,Data!B:B,0))</f>
         <v>E07000191</v>
       </c>
+      <c r="C14">
+        <v>201718</v>
+      </c>
+      <c r="D14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" t="s">
+        <v>75</v>
+      </c>
       <c r="F14" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+      <c r="I14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>63</v>
       </c>
-      <c r="B15">
-        <v>201718</v>
-      </c>
-      <c r="C15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" t="str">
+      <c r="B15" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A15,Data!B:B,0))</f>
         <v>E07000053</v>
       </c>
+      <c r="C15">
+        <v>201718</v>
+      </c>
+      <c r="D15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" t="s">
+        <v>74</v>
+      </c>
       <c r="F15" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+      <c r="I15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>37</v>
       </c>
-      <c r="B16">
-        <v>201819</v>
-      </c>
-      <c r="C16" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" t="str">
+      <c r="B16" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A16,Data!B:B,0))</f>
         <v>E07000004</v>
       </c>
+      <c r="C16">
+        <v>201819</v>
+      </c>
+      <c r="D16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" t="s">
+        <v>82</v>
+      </c>
       <c r="F16" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+      <c r="I16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>39</v>
       </c>
-      <c r="B17">
-        <v>201819</v>
-      </c>
-      <c r="C17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" t="s">
-        <v>84</v>
-      </c>
-      <c r="E17" t="str">
+      <c r="B17" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A17,Data!B:B,0))</f>
         <v>E07000005</v>
       </c>
+      <c r="C17">
+        <v>201819</v>
+      </c>
+      <c r="D17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" t="s">
+        <v>82</v>
+      </c>
       <c r="F17" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+      <c r="I17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>41</v>
       </c>
-      <c r="B18">
-        <v>201819</v>
-      </c>
-      <c r="C18" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" t="str">
+      <c r="B18" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A18,Data!B:B,0))</f>
         <v>E07000006</v>
       </c>
+      <c r="C18">
+        <v>201819</v>
+      </c>
+      <c r="D18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" t="s">
+        <v>82</v>
+      </c>
       <c r="F18" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+      <c r="I18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>43</v>
       </c>
-      <c r="B19">
-        <v>201819</v>
-      </c>
-      <c r="C19" t="s">
-        <v>83</v>
-      </c>
-      <c r="D19" t="s">
-        <v>84</v>
-      </c>
-      <c r="E19" t="str">
+      <c r="B19" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A19,Data!B:B,0))</f>
         <v>E07000007</v>
       </c>
+      <c r="C19">
+        <v>201819</v>
+      </c>
+      <c r="D19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" t="s">
+        <v>82</v>
+      </c>
       <c r="F19" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+      <c r="I19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>8</v>
       </c>
-      <c r="B20">
-        <v>201920</v>
-      </c>
-      <c r="C20" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E20" t="str">
+      <c r="B20" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A20,Data!B:B,0))</f>
         <v>E07000150</v>
       </c>
+      <c r="C20">
+        <v>201920</v>
+      </c>
+      <c r="D20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" t="s">
+        <v>86</v>
+      </c>
       <c r="F20" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+      <c r="I20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="B21">
-        <v>201920</v>
-      </c>
-      <c r="C21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E21" t="str">
+      <c r="B21" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A21,Data!B:B,0))</f>
         <v>E07000151</v>
       </c>
+      <c r="C21">
+        <v>201920</v>
+      </c>
+      <c r="D21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E21" t="s">
+        <v>86</v>
+      </c>
       <c r="F21" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+      <c r="I21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="B22">
-        <v>201920</v>
-      </c>
-      <c r="C22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E22" t="str">
+      <c r="B22" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A22,Data!B:B,0))</f>
         <v>E07000152</v>
       </c>
+      <c r="C22">
+        <v>201920</v>
+      </c>
+      <c r="D22" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" t="s">
+        <v>86</v>
+      </c>
       <c r="F22" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+      <c r="I22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
-        <v>201920</v>
-      </c>
-      <c r="C23" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E23" t="str">
+      <c r="B23" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A23,Data!B:B,0))</f>
         <v>E07000153</v>
       </c>
+      <c r="C23">
+        <v>201920</v>
+      </c>
+      <c r="D23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" t="s">
+        <v>86</v>
+      </c>
       <c r="F23" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+      <c r="I23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24">
-        <v>201920</v>
-      </c>
-      <c r="C24" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" t="s">
-        <v>88</v>
-      </c>
-      <c r="E24" t="str">
+      <c r="B24" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A24,Data!B:B,0))</f>
         <v>E07000154</v>
       </c>
+      <c r="C24">
+        <v>201920</v>
+      </c>
+      <c r="D24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" t="s">
+        <v>86</v>
+      </c>
       <c r="F24" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+      <c r="I24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>25</v>
       </c>
-      <c r="B25">
-        <v>201920</v>
-      </c>
-      <c r="C25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" t="str">
+      <c r="B25" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A25,Data!B:B,0))</f>
         <v>E07000155</v>
       </c>
+      <c r="C25">
+        <v>201920</v>
+      </c>
+      <c r="D25" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" t="s">
+        <v>86</v>
+      </c>
       <c r="F25" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+      <c r="I25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="B26">
-        <v>201920</v>
-      </c>
-      <c r="C26" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" t="str">
+      <c r="B26" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A26,Data!B:B,0))</f>
         <v>E07000156</v>
       </c>
+      <c r="C26">
+        <v>201920</v>
+      </c>
+      <c r="D26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" t="s">
+        <v>86</v>
+      </c>
       <c r="F26" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+      <c r="I26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27">
+        <v>202122</v>
+      </c>
+      <c r="E27" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" t="s">
+        <v>105</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I27" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28">
+        <v>202122</v>
+      </c>
+      <c r="E28" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" t="s">
+        <v>105</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B27">
+      <c r="C29">
         <v>202122</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E29" t="s">
+        <v>105</v>
+      </c>
+      <c r="F29" t="s">
+        <v>105</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30">
+        <v>202122</v>
+      </c>
+      <c r="E30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" t="s">
+        <v>105</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H30" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="I30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31">
+        <v>202122</v>
+      </c>
+      <c r="E31" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" t="s">
+        <v>105</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H31" s="6" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>99</v>
-      </c>
-      <c r="B28">
+      <c r="I31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32">
         <v>202122</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H32" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F28" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B29">
-        <v>202122</v>
-      </c>
-      <c r="C29" t="s">
-        <v>108</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B30">
-        <v>202122</v>
-      </c>
-      <c r="C30" t="s">
-        <v>108</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="F30" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B31">
-        <v>202122</v>
-      </c>
-      <c r="C31" t="s">
-        <v>108</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F31" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32">
-        <v>202122</v>
-      </c>
-      <c r="C32" t="s">
-        <v>108</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F32" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="I32" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>65</v>
       </c>
-      <c r="B33">
-        <v>201718</v>
-      </c>
-      <c r="C33">
-        <f>SUMIFS(Data!H:H,Data!A:A,LADs!B33,Data!B:B,LADs!A33)</f>
-        <v>39600</v>
-      </c>
-      <c r="E33" t="str">
+      <c r="B33" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A33,Data!B:B,0))</f>
         <v>z</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <v>201718</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>65</v>
       </c>
-      <c r="B34">
-        <v>201819</v>
-      </c>
-      <c r="C34">
-        <f>SUMIFS(Data!H:H,Data!A:A,LADs!B34,Data!B:B,LADs!A34)</f>
-        <v>32930</v>
-      </c>
-      <c r="E34" t="str">
+      <c r="B34" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A34,Data!B:B,0))</f>
         <v>z</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C34">
+        <v>201819</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>65</v>
       </c>
-      <c r="B35">
-        <v>201920</v>
-      </c>
-      <c r="C35">
-        <f>SUMIFS(Data!H:H,Data!A:A,LADs!B35,Data!B:B,LADs!A35)</f>
-        <v>7230</v>
-      </c>
-      <c r="E35" t="str">
+      <c r="B35" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A35,Data!B:B,0))</f>
         <v>z</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C35">
+        <v>201920</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>65</v>
       </c>
-      <c r="B36">
-        <v>202021</v>
-      </c>
-      <c r="C36">
-        <f>SUMIFS(Data!H:H,Data!A:A,LADs!B36,Data!B:B,LADs!A36)</f>
-        <v>7200</v>
-      </c>
-      <c r="E36" t="str">
+      <c r="B36" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A36,Data!B:B,0))</f>
         <v>z</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C36">
+        <v>202021</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>65</v>
       </c>
-      <c r="B37">
-        <v>202122</v>
-      </c>
-      <c r="C37">
-        <f>SUMIFS(Data!H:H,Data!A:A,LADs!B37,Data!B:B,LADs!A37)</f>
-        <v>2460</v>
-      </c>
-      <c r="E37" t="str">
+      <c r="B37" t="str">
         <f>INDEX(Data!C:C,MATCH(LADs!A37,Data!B:B,0))</f>
         <v>z</v>
       </c>
+      <c r="C37">
+        <v>202122</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D33" xr:uid="{63CCF82A-C657-4D4C-8BFB-87C91102109C}"/>
+  <autoFilter ref="A1:E33" xr:uid="{63CCF82A-C657-4D4C-8BFB-87C91102109C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -9302,26 +9454,26 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to new lsip names update to latest LAs make dashboard work with the new ILR data at LEP and LSIP level tify code version control
</commit_message>
<xml_diff>
--- a/Data/1-2_LEPmissing/missing_leps.xlsx
+++ b/Data/1-2_LEPmissing/missing_leps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://educationgovuk-my.sharepoint.com/personal/paul_james_education_gov_uk/Documents/Documents/RProjects/lsip_dashboard/Data/1-2_LEPmissing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{FFE31EE7-898F-4126-9D75-02FABA5FEDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9ED972DF-E4B2-45E8-88A1-A2D756D8276C}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="8_{FFE31EE7-898F-4126-9D75-02FABA5FEDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E1577DA-9403-405F-8BF4-DEC1D8CA288B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="1" xr2:uid="{1E32C2D0-1FE1-4979-B264-7DA23B5223C8}"/>
   </bookViews>
@@ -267,9 +267,6 @@
     <t>Dorset</t>
   </si>
   <si>
-    <t>Heart of South West</t>
-  </si>
-  <si>
     <t>where to find it on the map</t>
   </si>
   <si>
@@ -394,6 +391,9 @@
   </si>
   <si>
     <t>Lookup</t>
+  </si>
+  <si>
+    <t>Heart of the South West</t>
   </si>
 </sst>
 </file>
@@ -8559,8 +8559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63CCF82A-C657-4D4C-8BFB-87C91102109C}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27:I32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8573,31 +8573,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>67</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -8618,10 +8618,10 @@
         <v>73</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -8642,10 +8642,10 @@
         <v>73</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -8666,10 +8666,10 @@
         <v>73</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -8690,10 +8690,10 @@
         <v>73</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -8708,7 +8708,7 @@
         <v>201718</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
         <v>74</v>
@@ -8717,7 +8717,7 @@
         <v>74</v>
       </c>
       <c r="I6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -8732,7 +8732,7 @@
         <v>201718</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E7" t="s">
         <v>74</v>
@@ -8741,7 +8741,7 @@
         <v>74</v>
       </c>
       <c r="I7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -8756,7 +8756,7 @@
         <v>201718</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E8" t="s">
         <v>74</v>
@@ -8765,7 +8765,7 @@
         <v>74</v>
       </c>
       <c r="I8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -8780,7 +8780,7 @@
         <v>201718</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E9" t="s">
         <v>74</v>
@@ -8789,7 +8789,7 @@
         <v>74</v>
       </c>
       <c r="I9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -8804,7 +8804,7 @@
         <v>201718</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E10" t="s">
         <v>74</v>
@@ -8813,7 +8813,7 @@
         <v>74</v>
       </c>
       <c r="I10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -8828,7 +8828,7 @@
         <v>201718</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E11" t="s">
         <v>74</v>
@@ -8837,7 +8837,7 @@
         <v>74</v>
       </c>
       <c r="I11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -8852,16 +8852,16 @@
         <v>201718</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -8876,7 +8876,7 @@
         <v>201718</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E13" t="s">
         <v>74</v>
@@ -8885,7 +8885,7 @@
         <v>74</v>
       </c>
       <c r="I13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -8900,16 +8900,16 @@
         <v>201718</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -8924,7 +8924,7 @@
         <v>201718</v>
       </c>
       <c r="D15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E15" t="s">
         <v>74</v>
@@ -8933,7 +8933,7 @@
         <v>74</v>
       </c>
       <c r="I15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -8948,16 +8948,16 @@
         <v>201819</v>
       </c>
       <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
         <v>81</v>
       </c>
-      <c r="E16" t="s">
-        <v>82</v>
-      </c>
       <c r="F16" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -8972,16 +8972,16 @@
         <v>201819</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -8996,16 +8996,16 @@
         <v>201819</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -9020,16 +9020,16 @@
         <v>201819</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -9044,16 +9044,16 @@
         <v>201920</v>
       </c>
       <c r="D20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -9068,16 +9068,16 @@
         <v>201920</v>
       </c>
       <c r="D21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -9092,16 +9092,16 @@
         <v>201920</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -9116,16 +9116,16 @@
         <v>201920</v>
       </c>
       <c r="D23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -9140,16 +9140,16 @@
         <v>201920</v>
       </c>
       <c r="D24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -9164,16 +9164,16 @@
         <v>201920</v>
       </c>
       <c r="D25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I25" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -9188,172 +9188,172 @@
         <v>201920</v>
       </c>
       <c r="D26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C27">
         <v>202122</v>
       </c>
       <c r="E27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G27" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="H27" s="6" t="s">
-        <v>110</v>
-      </c>
       <c r="I27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28">
         <v>202122</v>
       </c>
       <c r="E28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G28" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H28" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="H28" s="6" t="s">
-        <v>110</v>
-      </c>
       <c r="I28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C29">
         <v>202122</v>
       </c>
       <c r="E29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G29" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H29" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="H29" s="6" t="s">
-        <v>110</v>
-      </c>
       <c r="I29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C30">
         <v>202122</v>
       </c>
       <c r="E30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G30" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H30" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="H30" s="6" t="s">
-        <v>108</v>
-      </c>
       <c r="I30" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C31">
         <v>202122</v>
       </c>
       <c r="E31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G31" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H31" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="H31" s="6" t="s">
-        <v>108</v>
-      </c>
       <c r="I31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32">
         <v>202122</v>
       </c>
       <c r="E32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G32" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H32" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="H32" s="6" t="s">
-        <v>108</v>
-      </c>
       <c r="I32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -9454,26 +9454,26 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>